<commit_message>
Personnels logic JUST DRAFT
</commit_message>
<xml_diff>
--- a/test_models/users.xlsx
+++ b/test_models/users.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo17\PycharmProjects\FlaskBasic\test_models\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12075"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12072"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -66,7 +71,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -383,7 +388,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -391,18 +396,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="N1" activeCellId="1" sqref="L2 N1:N1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="11" max="11" width="18.7109375" customWidth="1"/>
+    <col min="11" max="11" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -436,8 +441,11 @@
       <c r="K1" t="s">
         <v>12</v>
       </c>
+      <c r="L1">
+        <v>1</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -470,6 +478,9 @@
       </c>
       <c r="K2" t="s">
         <v>13</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Personnels in DB now working
</commit_message>
<xml_diff>
--- a/test_models/users.xlsx
+++ b/test_models/users.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo17\PycharmProjects\FlaskBasic\test_models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ANTON\PycharmProjects\FlaskBasic\test_models\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12072"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12075"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>имя</t>
   </si>
@@ -66,6 +66,21 @@
   </si>
   <si>
     <t>Не состоит в браке</t>
+  </si>
+  <si>
+    <t>фамилия 3</t>
+  </si>
+  <si>
+    <t>имя 3</t>
+  </si>
+  <si>
+    <t>отчество 3</t>
+  </si>
+  <si>
+    <t>another@email.com</t>
+  </si>
+  <si>
+    <t>qwerty1</t>
   </si>
 </sst>
 </file>
@@ -176,7 +191,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -211,7 +226,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -396,18 +411,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N1" activeCellId="1" sqref="L2 N1:N1048576"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="11" max="11" width="18.6640625" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -445,7 +460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -481,14 +496,53 @@
       </c>
       <c r="L2">
         <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3">
+        <v>1960</v>
+      </c>
+      <c r="E3">
+        <v>64</v>
+      </c>
+      <c r="F3">
+        <v>21</v>
+      </c>
+      <c r="G3">
+        <v>33</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L3">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H1" r:id="rId1"/>
     <hyperlink ref="H2" r:id="rId2"/>
+    <hyperlink ref="H3" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>